<commit_message>
Fixed power factory error and excel formula
</commit_message>
<xml_diff>
--- a/Power Factory Comparison.xlsx
+++ b/Power Factory Comparison.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Ia Ib Ic" sheetId="1" r:id="rId1"/>
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
-  <si>
-    <t>])</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
   <si>
     <t>Phase A magnitude</t>
   </si>
@@ -39,30 +36,12 @@
     <t>Phase C angle</t>
   </si>
   <si>
-    <t>Ia_pf = np.matrix([</t>
-  </si>
-  <si>
-    <t>Ib_pf = np.matrix([</t>
-  </si>
-  <si>
-    <t>Ic_pf = np.matrix([</t>
-  </si>
-  <si>
     <t>This can be used for both I and V components</t>
   </si>
   <si>
     <t xml:space="preserve">Open Power Factory results in this order and paste the results of Voltage and currents to get </t>
   </si>
   <si>
-    <t>Va_pf = np.matrix([</t>
-  </si>
-  <si>
-    <t>Vb_pf = np.matrix([</t>
-  </si>
-  <si>
-    <t>Vc_pf = np.matrix([</t>
-  </si>
-  <si>
     <t>Goto File - Options - Advanced - Use system seperators</t>
   </si>
   <si>
@@ -75,30 +54,9 @@
     <t>Slack Voltage</t>
   </si>
   <si>
-    <t>Ia_sl_pf = np.matrix([</t>
-  </si>
-  <si>
-    <t>Ib_sl_pf = np.matrix([</t>
-  </si>
-  <si>
-    <t>Ic_sl_pf = np.matrix([</t>
-  </si>
-  <si>
-    <t>Va_sl_pf = np.matrix([</t>
-  </si>
-  <si>
-    <t>Vb_sl_pf = np.matrix([</t>
-  </si>
-  <si>
-    <t>Vc_sl_pf = np.matrix([</t>
-  </si>
-  <si>
     <t>Sabc Slack</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Sabc_pq_sp =  np.matrix(   [</t>
   </si>
   <si>
@@ -108,9 +66,6 @@
     <t xml:space="preserve">                    ,dtype = np.complex </t>
   </si>
   <si>
-    <t xml:space="preserve">                    ) #kW and kVAr</t>
-  </si>
-  <si>
     <t>Sabc_sl_sp =  np.matrix(   [</t>
   </si>
   <si>
@@ -133,6 +88,21 @@
   </si>
   <si>
     <t>C, deg</t>
+  </si>
+  <si>
+    <t>Iabc_pq_pf =  np.matrix(   [</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                    ).T #kW and kVAr</t>
+  </si>
+  <si>
+    <t>Vabc_pq_pf =  np.matrix(   [</t>
+  </si>
+  <si>
+    <t>Iabc_sl_pf =  np.matrix(   [</t>
+  </si>
+  <si>
+    <t>Vabc_sl_pf =  np.matrix(   [</t>
   </si>
 </sst>
 </file>
@@ -477,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:L14"/>
+  <dimension ref="A2:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3:L7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,160 +463,161 @@
     <col min="6" max="6" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="G3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>0.85361334927999999</v>
+        <v>0.86676467552000003</v>
       </c>
       <c r="B4" s="1">
-        <v>-22.597021296000001</v>
+        <v>-23.168007119999999</v>
       </c>
       <c r="C4" s="1">
-        <v>1.609734392</v>
+        <v>1.6143920469999999</v>
       </c>
       <c r="D4" s="1">
-        <v>-158.13889773</v>
+        <v>-158.37122826000001</v>
       </c>
       <c r="E4" s="1">
-        <v>0.31635572983999999</v>
+        <v>0.31071857716000001</v>
       </c>
       <c r="F4" s="1">
-        <v>107.76170403</v>
+        <v>108.46692830000001</v>
       </c>
       <c r="H4" t="str">
-        <f>CONCATENATE("[",A4,"*np.exp(1j*np.deg2rad(",B4,"))],")</f>
-        <v>[0.85361334928*np.exp(1j*np.deg2rad(-22.597021296))],</v>
+        <f>CONCATENATE("[",A4,"*np.exp(1j*np.deg2rad(",B4,")),")</f>
+        <v>[0.86676467552*np.exp(1j*np.deg2rad(-23.16800712)),</v>
       </c>
       <c r="J4" t="str">
-        <f>CONCATENATE("[",C4,"*np.exp(1j*np.deg2rad(",D4,"))],")</f>
-        <v>[1.609734392*np.exp(1j*np.deg2rad(-158.13889773))],</v>
+        <f>CONCATENATE(C4,"*np.exp(1j*np.deg2rad(",D4,")),")</f>
+        <v>1.614392047*np.exp(1j*np.deg2rad(-158.37122826)),</v>
       </c>
       <c r="L4" t="str">
-        <f>CONCATENATE("[",E4,"*np.exp(1j*np.deg2rad(",F4,"))],")</f>
-        <v>[0.31635572984*np.exp(1j*np.deg2rad(107.76170403))],</v>
+        <f>CONCATENATE(E4,"*np.exp(1j*np.deg2rad(",F4,"))],")</f>
+        <v>0.31071857716*np.exp(1j*np.deg2rad(108.4669283))],</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>1.1217345202</v>
+        <v>1.1387494998000001</v>
       </c>
       <c r="B5" s="1">
-        <v>-45.833804321000002</v>
+        <v>-46.403411358</v>
       </c>
       <c r="C5" s="1">
-        <v>0.28984573029999999</v>
+        <v>0.29070024235000003</v>
       </c>
       <c r="D5" s="1">
-        <v>-177.53818591000001</v>
+        <v>-177.76002958000001</v>
       </c>
       <c r="E5" s="1">
-        <v>0.17162062815000001</v>
+        <v>0.16859090052</v>
       </c>
       <c r="F5" s="1">
-        <v>95.275718806</v>
+        <v>95.969503626999995</v>
       </c>
       <c r="H5" t="str">
-        <f t="shared" ref="H5" si="0">CONCATENATE("[",A5,"*np.exp(1j*np.deg2rad(",B5,"))],")</f>
-        <v>[1.1217345202*np.exp(1j*np.deg2rad(-45.833804321))],</v>
+        <f t="shared" ref="H5:H6" si="0">CONCATENATE("[",A5,"*np.exp(1j*np.deg2rad(",B5,")),")</f>
+        <v>[1.1387494998*np.exp(1j*np.deg2rad(-46.403411358)),</v>
       </c>
       <c r="J5" t="str">
-        <f t="shared" ref="J5" si="1">CONCATENATE("[",C5,"*np.exp(1j*np.deg2rad(",D5,"))],")</f>
-        <v>[0.2898457303*np.exp(1j*np.deg2rad(-177.53818591))],</v>
+        <f t="shared" ref="J5:J6" si="1">CONCATENATE(C5,"*np.exp(1j*np.deg2rad(",D5,")),")</f>
+        <v>0.29070024235*np.exp(1j*np.deg2rad(-177.76002958)),</v>
       </c>
       <c r="L5" t="str">
-        <f t="shared" ref="L5" si="2">CONCATENATE("[",E5,"*np.exp(1j*np.deg2rad(",F5,"))],")</f>
-        <v>[0.17162062815*np.exp(1j*np.deg2rad(95.275718806))],</v>
+        <f t="shared" ref="L5:L6" si="2">CONCATENATE(E5,"*np.exp(1j*np.deg2rad(",F5,"))],")</f>
+        <v>0.16859090052*np.exp(1j*np.deg2rad(95.969503627))],</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>0.54690896501999997</v>
+        <v>0.86693887871999997</v>
       </c>
       <c r="B6" s="1">
-        <v>-2.4474461726999999</v>
+        <v>-23.183031658000001</v>
       </c>
       <c r="C6" s="1">
-        <v>0.90680096195000004</v>
+        <v>1.0204854981</v>
       </c>
       <c r="D6" s="1">
-        <v>-137.21052139</v>
+        <v>-139.95476823999999</v>
       </c>
       <c r="E6" s="1">
-        <v>0.65033987737999999</v>
+        <v>0.16851041836</v>
       </c>
       <c r="F6" s="1">
-        <v>79.452062479999995</v>
+        <v>95.960819649000001</v>
       </c>
       <c r="H6" t="str">
-        <f>CONCATENATE("[",A6,"*np.exp(1j*np.deg2rad(",B6,"))]")</f>
-        <v>[0.54690896502*np.exp(1j*np.deg2rad(-2.4474461727))]</v>
+        <f t="shared" si="0"/>
+        <v>[0.86693887872*np.exp(1j*np.deg2rad(-23.183031658)),</v>
       </c>
       <c r="J6" t="str">
-        <f>CONCATENATE("[",C6,"*np.exp(1j*np.deg2rad(",D6,"))]")</f>
-        <v>[0.90680096195*np.exp(1j*np.deg2rad(-137.21052139))]</v>
+        <f t="shared" si="1"/>
+        <v>1.0204854981*np.exp(1j*np.deg2rad(-139.95476824)),</v>
       </c>
       <c r="L6" t="str">
-        <f>CONCATENATE("[",E6,"*np.exp(1j*np.deg2rad(",F6,"))]")</f>
-        <v>[0.65033987738*np.exp(1j*np.deg2rad(79.45206248))]</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G7" t="s">
-        <v>0</v>
-      </c>
-      <c r="J7" t="s">
-        <v>0</v>
-      </c>
-      <c r="L7" t="s">
-        <v>0</v>
+        <f>CONCATENATE(E6,"*np.exp(1j*np.deg2rad(",F6,"))]")</f>
+        <v>0.16851041836*np.exp(1j*np.deg2rad(95.960819649))]</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="I10" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -657,10 +628,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:L9"/>
+  <dimension ref="A4:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5:L9"/>
+      <selection activeCell="G4" sqref="G4:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,140 +644,143 @@
     <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+    </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="G5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>63.086698579999997</v>
+        <v>62.129490959000002</v>
       </c>
       <c r="B6">
-        <v>-0.79561180899999995</v>
+        <v>-1.3665976339999999</v>
       </c>
       <c r="C6">
-        <v>62.122049758999999</v>
+        <v>61.942822493000001</v>
       </c>
       <c r="D6">
-        <v>-121.269000085</v>
+        <v>-121.501330612</v>
       </c>
       <c r="E6">
-        <v>65.165654304</v>
+        <v>66.347909791999996</v>
       </c>
       <c r="F6">
-        <v>121.797947494</v>
+        <v>122.503171764</v>
       </c>
       <c r="H6" t="str">
-        <f>CONCATENATE("[",A6,"*np.exp(1j*np.deg2rad(",B6,"))],")</f>
-        <v>[63.08669858*np.exp(1j*np.deg2rad(-0.795611809))],</v>
+        <f>CONCATENATE("[",A6,"*np.exp(1j*np.deg2rad(",B6,")),")</f>
+        <v>[62.129490959*np.exp(1j*np.deg2rad(-1.366597634)),</v>
       </c>
       <c r="J6" t="str">
-        <f>CONCATENATE("[",C6,"*np.exp(1j*np.deg2rad(",D6,"))],")</f>
-        <v>[62.122049759*np.exp(1j*np.deg2rad(-121.269000085))],</v>
+        <f>CONCATENATE(C6,"*np.exp(1j*np.deg2rad(",D6,")),")</f>
+        <v>61.942822493*np.exp(1j*np.deg2rad(-121.501330612)),</v>
       </c>
       <c r="L6" t="str">
-        <f>CONCATENATE("[",E6,"*np.exp(1j*np.deg2rad(",F6,"))],")</f>
-        <v>[65.165654304*np.exp(1j*np.deg2rad(121.797947494))],</v>
+        <f>CONCATENATE(E6,"*np.exp(1j*np.deg2rad(",F6,"))],")</f>
+        <v>66.347909792*np.exp(1j*np.deg2rad(122.503171764))],</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>63.036910108999997</v>
+        <v>62.095024524999999</v>
       </c>
       <c r="B7">
-        <v>-0.83380432100000001</v>
+        <v>-1.4034113580000001</v>
       </c>
       <c r="C7">
-        <v>62.197764161999999</v>
+        <v>62.014934117999999</v>
       </c>
       <c r="D7">
-        <v>-121.228253434</v>
+        <v>-121.450097103</v>
       </c>
       <c r="E7">
-        <v>65.145664643000003</v>
+        <v>66.316389870999998</v>
       </c>
       <c r="F7">
-        <v>121.840769983</v>
+        <v>122.534554804</v>
       </c>
       <c r="H7" t="str">
-        <f t="shared" ref="H7" si="0">CONCATENATE("[",A7,"*np.exp(1j*np.deg2rad(",B7,"))],")</f>
-        <v>[63.036910109*np.exp(1j*np.deg2rad(-0.833804321))],</v>
+        <f t="shared" ref="H7:H8" si="0">CONCATENATE("[",A7,"*np.exp(1j*np.deg2rad(",B7,")),")</f>
+        <v>[62.095024525*np.exp(1j*np.deg2rad(-1.403411358)),</v>
       </c>
       <c r="J7" t="str">
-        <f t="shared" ref="J7" si="1">CONCATENATE("[",C7,"*np.exp(1j*np.deg2rad(",D7,"))],")</f>
-        <v>[62.197764162*np.exp(1j*np.deg2rad(-121.228253434))],</v>
+        <f t="shared" ref="J7:J8" si="1">CONCATENATE(C7,"*np.exp(1j*np.deg2rad(",D7,")),")</f>
+        <v>62.014934118*np.exp(1j*np.deg2rad(-121.450097103)),</v>
       </c>
       <c r="L7" t="str">
-        <f t="shared" ref="L7" si="2">CONCATENATE("[",E7,"*np.exp(1j*np.deg2rad(",F7,"))],")</f>
-        <v>[65.145664643*np.exp(1j*np.deg2rad(121.840769983))],</v>
+        <f t="shared" ref="L7:L8" si="2">CONCATENATE(E7,"*np.exp(1j*np.deg2rad(",F7,"))],")</f>
+        <v>66.316389871*np.exp(1j*np.deg2rad(122.534554804))],</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>63.141370330000001</v>
+        <v>62.117006623000002</v>
       </c>
       <c r="B8" s="1">
-        <v>-0.82125691000000001</v>
+        <v>-1.3816221719999999</v>
       </c>
       <c r="C8" s="1">
-        <v>62.154586369</v>
+        <v>61.975945099</v>
       </c>
       <c r="D8" s="1">
-        <v>-121.239876724</v>
+        <v>-121.519819412</v>
       </c>
       <c r="E8" s="1">
-        <v>65.098044778000002</v>
+        <v>66.348063199999999</v>
       </c>
       <c r="F8" s="1">
-        <v>121.78828015800001</v>
+        <v>122.525870826</v>
       </c>
       <c r="H8" t="str">
-        <f t="shared" ref="H8" si="3">CONCATENATE("[",A8,"*np.exp(1j*np.deg2rad(",B8,"))],")</f>
-        <v>[63.14137033*np.exp(1j*np.deg2rad(-0.82125691))],</v>
+        <f t="shared" si="0"/>
+        <v>[62.117006623*np.exp(1j*np.deg2rad(-1.381622172)),</v>
       </c>
       <c r="J8" t="str">
-        <f t="shared" ref="J8" si="4">CONCATENATE("[",C8,"*np.exp(1j*np.deg2rad(",D8,"))],")</f>
-        <v>[62.154586369*np.exp(1j*np.deg2rad(-121.239876724))],</v>
+        <f t="shared" si="1"/>
+        <v>61.975945099*np.exp(1j*np.deg2rad(-121.519819412)),</v>
       </c>
       <c r="L8" t="str">
-        <f t="shared" ref="L8" si="5">CONCATENATE("[",E8,"*np.exp(1j*np.deg2rad(",F8,"))],")</f>
-        <v>[65.098044778*np.exp(1j*np.deg2rad(121.788280158))],</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G9" t="s">
-        <v>0</v>
-      </c>
-      <c r="J9" t="s">
-        <v>0</v>
-      </c>
-      <c r="L9" t="s">
-        <v>0</v>
+        <f>CONCATENATE(E8,"*np.exp(1j*np.deg2rad(",F8,"))]")</f>
+        <v>66.3480632*np.exp(1j*np.deg2rad(122.525870826))]</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -818,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:M35"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,249 +803,246 @@
   <sheetData>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="M5" s="1"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2.4027562640000002</v>
+        <v>2.8069821840000002</v>
       </c>
       <c r="B6">
-        <v>-28.263023464</v>
+        <v>-32.037382293</v>
       </c>
       <c r="C6">
-        <v>2.7300489529999998</v>
+        <v>2.8561766400000002</v>
       </c>
       <c r="D6">
-        <v>-153.05331253</v>
+        <v>-153.54689552799999</v>
       </c>
       <c r="E6">
-        <v>1.1016383240000001</v>
+        <v>0.63750314299999999</v>
       </c>
       <c r="F6">
-        <v>90.480307238999998</v>
+        <v>103.573568845</v>
       </c>
       <c r="I6" t="str">
-        <f>CONCATENATE("[",A6,"*np.exp(1j*np.deg2rad(",B6,"))],")</f>
-        <v>[2.402756264*np.exp(1j*np.deg2rad(-28.263023464))],</v>
+        <f>CONCATENATE("[",A6,"*np.exp(1j*np.deg2rad(",B6,")),")</f>
+        <v>[2.806982184*np.exp(1j*np.deg2rad(-32.037382293)),</v>
       </c>
       <c r="K6" t="str">
-        <f>CONCATENATE("[",C6,"*np.exp(1j*np.deg2rad(",D6,"))],")</f>
-        <v>[2.730048953*np.exp(1j*np.deg2rad(-153.05331253))],</v>
+        <f>CONCATENATE(C6,"*np.exp(1j*np.deg2rad(",D6,")),")</f>
+        <v>2.85617664*np.exp(1j*np.deg2rad(-153.546895528)),</v>
       </c>
       <c r="M6" t="str">
-        <f>CONCATENATE("[",E6,"*np.exp(1j*np.deg2rad(",F6,"))],")</f>
-        <v>[1.101638324*np.exp(1j*np.deg2rad(90.480307239))],</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I7" t="s">
-        <v>0</v>
-      </c>
-      <c r="K7" t="s">
-        <v>0</v>
-      </c>
-      <c r="M7" t="s">
-        <v>0</v>
+        <f>CONCATENATE(E6,"*np.exp(1j*np.deg2rad(",F6,"))]")</f>
+        <v>0.637503143*np.exp(1j*np.deg2rad(103.573568845))]</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="F13" t="s">
-        <v>38</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M13" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="H13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K13" s="1"/>
+      <c r="M13" s="1"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>63.212039279999999</v>
+        <v>62.292804335</v>
       </c>
       <c r="B14">
-        <v>-0.76941527799999998</v>
+        <v>-1.3361216579999999</v>
       </c>
       <c r="C14">
-        <v>62.242151767999999</v>
+        <v>62.055452267</v>
       </c>
       <c r="D14">
-        <v>-121.114993036</v>
+        <v>-121.32169707600001</v>
       </c>
       <c r="E14">
-        <v>65.121473346000002</v>
+        <v>66.273554938000004</v>
       </c>
       <c r="F14">
-        <v>121.812761909</v>
+        <v>122.49400607299999</v>
       </c>
       <c r="I14" t="str">
-        <f>CONCATENATE("[",A14,"*np.exp(1j*np.deg2rad(",B14,"))],")</f>
-        <v>[63.21203928*np.exp(1j*np.deg2rad(-0.769415278))],</v>
+        <f>CONCATENATE("[",A14,"*np.exp(1j*np.deg2rad(",B14,")),")</f>
+        <v>[62.292804335*np.exp(1j*np.deg2rad(-1.336121658)),</v>
       </c>
       <c r="K14" t="str">
-        <f>CONCATENATE("[",C14,"*np.exp(1j*np.deg2rad(",D14,"))],")</f>
-        <v>[62.242151768*np.exp(1j*np.deg2rad(-121.114993036))],</v>
+        <f>CONCATENATE(C14,"*np.exp(1j*np.deg2rad(",D14,")),")</f>
+        <v>62.055452267*np.exp(1j*np.deg2rad(-121.321697076)),</v>
       </c>
       <c r="M14" t="str">
-        <f>CONCATENATE("[",E14,"*np.exp(1j*np.deg2rad(",F14,"))],")</f>
-        <v>[65.121473346*np.exp(1j*np.deg2rad(121.812761909))],</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I15" t="s">
-        <v>0</v>
-      </c>
-      <c r="K15" t="s">
-        <v>0</v>
-      </c>
-      <c r="M15" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+        <f>CONCATENATE(E14,"*np.exp(1j*np.deg2rad(",F14,"))]")</f>
+        <v>66.273554938*np.exp(1j*np.deg2rad(122.494006073))]</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>150.34732586000001</v>
+      </c>
+      <c r="B21">
+        <v>89.274183692999998</v>
+      </c>
+      <c r="C21">
+        <v>149.93885263000001</v>
+      </c>
+      <c r="D21">
+        <v>94.513653203000004</v>
+      </c>
+      <c r="E21">
+        <v>39.966843513000001</v>
+      </c>
+      <c r="F21">
+        <v>13.699638139999999</v>
+      </c>
+      <c r="I21" t="str">
+        <f>CONCATENATE("[",A21,"*1000+",B21,"*1000j ,")</f>
+        <v>[150.34732586*1000+89.274183693*1000j ,</v>
+      </c>
+      <c r="K21" t="str">
+        <f>CONCATENATE(C21,"*1000+",D21,"*1000j,")</f>
+        <v>149.93885263*1000+94.513653203*1000j,</v>
+      </c>
+      <c r="M21" t="str">
+        <f>CONCATENATE(E21,"*1000+",F21,"*1000j],")</f>
+        <v>39.966843513*1000+13.69963814*1000j],</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G20" t="s">
-        <v>31</v>
-      </c>
-      <c r="H20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>134.72979874999999</v>
-      </c>
-      <c r="B21">
-        <v>70.116791813000006</v>
-      </c>
-      <c r="C21">
-        <v>144.20068114</v>
-      </c>
-      <c r="D21">
-        <v>89.890881393000001</v>
-      </c>
-      <c r="E21">
-        <v>61.278020632999997</v>
-      </c>
-      <c r="F21">
-        <v>37.305178871999999</v>
-      </c>
-      <c r="H21" t="str">
-        <f>CONCATENATE("[",A21,"*1000+",B21,"*1000j],")</f>
-        <v>[134.72979875*1000+70.116791813*1000j],</v>
-      </c>
-      <c r="J21" t="str">
-        <f>CONCATENATE("[",C21,"*1000+",D21,"*1000j],")</f>
-        <v>[144.20068114*1000+89.890881393*1000j],</v>
-      </c>
-      <c r="L21" t="str">
-        <f>CONCATENATE("[",E21,"*1000+",F21,"*1000j]")</f>
-        <v>[61.278020633*1000+37.305178872*1000j]</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G23" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G24" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="G28" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>49.999999999000003</v>
+        <v>50</v>
       </c>
       <c r="B30" s="2">
         <v>20</v>
       </c>
       <c r="C30" s="2">
-        <v>79.999999998000007</v>
+        <v>79.999999998999996</v>
       </c>
       <c r="D30" s="2">
-        <v>59.999999999000003</v>
+        <v>60</v>
       </c>
       <c r="E30" s="2">
         <v>20</v>
       </c>
       <c r="F30" s="2">
-        <v>5</v>
+        <v>5.0000000001</v>
       </c>
       <c r="H30" t="str">
         <f>CONCATENATE("[",A30,"*1000+",B30,"*1000j ,")</f>
-        <v>[49.999999999*1000+20*1000j ,</v>
+        <v>[50*1000+20*1000j ,</v>
       </c>
       <c r="J30" t="str">
         <f>CONCATENATE(C30,"*1000+",D30,"*1000j,")</f>
-        <v>79.999999998*1000+59.999999999*1000j,</v>
+        <v>79.999999999*1000+60*1000j,</v>
       </c>
       <c r="L30" t="str">
         <f>CONCATENATE(E30,"*1000+",F30,"*1000j],")</f>
-        <v>20*1000+5*1000j],</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+        <v>20*1000+5.0000000001*1000j],</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>49.999999999000003</v>
+        <v>50</v>
       </c>
       <c r="B31" s="2">
-        <v>49.999999999000003</v>
+        <v>50</v>
       </c>
       <c r="C31" s="2">
-        <v>9.9999999997</v>
+        <v>9.9999999998</v>
       </c>
       <c r="D31" s="2">
         <v>15</v>
@@ -1080,66 +1051,66 @@
         <v>10</v>
       </c>
       <c r="F31" s="2">
-        <v>5</v>
+        <v>5.0000000001</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" ref="H31:H32" si="0">CONCATENATE("[",A31,"*1000+",B31,"*1000j ,")</f>
-        <v>[49.999999999*1000+49.999999999*1000j ,</v>
+        <v>[50*1000+50*1000j ,</v>
       </c>
       <c r="J31" t="str">
         <f>CONCATENATE(C31,"*1000+",D31,"*1000j,")</f>
-        <v>9.9999999997*1000+15*1000j,</v>
+        <v>9.9999999998*1000+15*1000j,</v>
       </c>
       <c r="L31" t="str">
         <f>CONCATENATE(E31,"*1000+",F31,"*1000j],")</f>
-        <v>10*1000+5*1000j],</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+        <v>10*1000+5.0000000001*1000j],</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>34.518673429000003</v>
+        <v>50</v>
       </c>
       <c r="B32" s="2">
-        <v>0.97998446796000005</v>
+        <v>20</v>
       </c>
       <c r="C32" s="2">
-        <v>54.186429087</v>
+        <v>59.999999999000003</v>
       </c>
       <c r="D32" s="2">
-        <v>15.507667957000001</v>
+        <v>20</v>
       </c>
       <c r="E32" s="2">
-        <v>31.294897484</v>
+        <v>10</v>
       </c>
       <c r="F32" s="2">
-        <v>28.512347575</v>
+        <v>5.0000000001</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="0"/>
-        <v>[34.518673429*1000+0.97998446796*1000j ,</v>
+        <v>[50*1000+20*1000j ,</v>
       </c>
       <c r="J32" t="str">
         <f>CONCATENATE(C32,"*1000+",D32,"*1000j,")</f>
-        <v>54.186429087*1000+15.507667957*1000j,</v>
+        <v>59.999999999*1000+20*1000j,</v>
       </c>
       <c r="L32" t="str">
         <f>CONCATENATE(E32,"*1000+",F32,"*1000j]")</f>
-        <v>31.294897484*1000+28.512347575*1000j]</v>
+        <v>10*1000+5.0000000001*1000j]</v>
       </c>
     </row>
     <row r="33" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I33" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I34" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I35" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>